<commit_message>
World Objects - Plants and Pickups
- Made all Plant Assets functionable
- Made all itemAssets (that's been made) functionable
- Added ColorMaterial functionability to plants
- Added a more smooth way to calculate the growth, updating each % per plant
</commit_message>
<xml_diff>
--- a/ProjectDocuments/Items_WorldObjects_Made.xlsx
+++ b/ProjectDocuments/Items_WorldObjects_Made.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Spill and Apps\Unity\Ørktantis\ProjectDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{3E1992FF-01F9-42C8-BCFB-9A2E261F9599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA2F638-346B-4328-87CB-0FEBF355904B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28770" yWindow="0" windowWidth="10365" windowHeight="15750"/>
+    <workbookView xWindow="28770" yWindow="0" windowWidth="10365" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="95">
   <si>
     <t>Plants</t>
   </si>
@@ -315,12 +315,18 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>TubePlastic</t>
+  </si>
+  <si>
+    <t>No.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -347,18 +353,47 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -367,12 +402,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,95 +729,162 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F83"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="2.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="2.77734375" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" customWidth="1"/>
-    <col min="6" max="6" width="2.77734375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="2.77734375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="4" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" customWidth="1"/>
+    <col min="7" max="7" width="2.77734375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G3" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="6">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G4" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="6">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G5" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G6" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="E7" t="s">
+      <c r="C7" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="6">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G7" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" t="s">
+      <c r="C8" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="6">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G8" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
+      <c r="C9" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="6">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G9" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="E10" t="s">
+      <c r="C10" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="6">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G10" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>11</v>
       </c>
@@ -782,369 +892,637 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="E12" t="s">
+      <c r="C12" s="3"/>
+      <c r="E12" s="4">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="E13" t="s">
+      <c r="C13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="4">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="E14" t="s">
+      <c r="C14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="4">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>15</v>
       </c>
-      <c r="E15" t="s">
+      <c r="C15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="6">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="G15" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="E16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="6">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="E17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C17" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="4">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="E19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="4">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>20</v>
       </c>
-      <c r="E20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="4">
+        <v>16</v>
+      </c>
+      <c r="F20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>21</v>
       </c>
-      <c r="E21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="4">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>22</v>
       </c>
-      <c r="E22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="4">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="E23" t="s">
+      <c r="C23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="4">
+        <v>19</v>
+      </c>
+      <c r="F23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E24" s="4">
+        <v>20</v>
+      </c>
+      <c r="F24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E25" s="4">
+        <v>21</v>
+      </c>
+      <c r="F25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E26" s="4">
+        <v>22</v>
+      </c>
+      <c r="F26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E27" s="4">
+        <v>23</v>
+      </c>
+      <c r="F27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E28" s="4">
+        <v>24</v>
+      </c>
+      <c r="F28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E29" s="4">
+        <v>25</v>
+      </c>
+      <c r="F29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E31" s="4">
+        <v>26</v>
+      </c>
+      <c r="F31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E32" s="4">
+        <v>27</v>
+      </c>
+      <c r="F32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E33" s="4">
+        <v>28</v>
+      </c>
+      <c r="F33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E34" s="4">
+        <v>29</v>
+      </c>
+      <c r="F34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E35" s="4">
+        <v>30</v>
+      </c>
+      <c r="F35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E36" s="4">
+        <v>31</v>
+      </c>
+      <c r="F36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E37" s="4">
+        <v>32</v>
+      </c>
+      <c r="F37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E38" s="4">
+        <v>33</v>
+      </c>
+      <c r="F38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E39" s="4">
+        <v>34</v>
+      </c>
+      <c r="F39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E41" s="6">
+        <v>35</v>
+      </c>
+      <c r="F41" t="s">
+        <v>58</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E42" s="6">
+        <v>36</v>
+      </c>
+      <c r="F42" t="s">
+        <v>59</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E43" s="6">
+        <v>37</v>
+      </c>
+      <c r="F43" t="s">
+        <v>60</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E44" s="6">
+        <v>38</v>
+      </c>
+      <c r="F44" t="s">
+        <v>61</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E45" s="6">
+        <v>39</v>
+      </c>
+      <c r="F45" t="s">
+        <v>2</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E46" s="4">
+        <v>40</v>
+      </c>
+      <c r="F46" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E47" s="6">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E24" t="s">
+      <c r="F47" t="s">
+        <v>93</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E49" s="4">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E25" t="s">
+      <c r="F49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E50" s="4">
         <v>43</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E26" t="s">
+      <c r="F50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E51" s="4">
         <v>44</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E27" t="s">
+      <c r="F51" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E52" s="4">
         <v>45</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E28" t="s">
+      <c r="F52" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E53" s="4">
         <v>46</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E29" t="s">
+      <c r="F53" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E54" s="4">
         <v>47</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E30" t="s">
+      <c r="F54" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E55" s="4">
         <v>48</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="E32" t="s">
+      <c r="F55" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E56" s="4">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E33" t="s">
+      <c r="F56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E57" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E34" t="s">
+      <c r="F57" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E58" s="4">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E35" t="s">
+      <c r="F58" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="59" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E59" s="4">
         <v>52</v>
       </c>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E36" t="s">
+      <c r="F59" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E60" s="4">
         <v>53</v>
       </c>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E37" t="s">
+      <c r="F60" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E61" s="4">
         <v>54</v>
       </c>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E38" t="s">
+      <c r="F61" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E62" s="4">
         <v>55</v>
       </c>
-    </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E39" t="s">
+      <c r="F62" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E64" s="6">
         <v>56</v>
       </c>
-    </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E40" t="s">
+      <c r="F64" t="s">
+        <v>3</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E65" s="6">
         <v>57</v>
       </c>
-    </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E42" t="s">
+      <c r="F65" t="s">
+        <v>77</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E66" s="6">
         <v>58</v>
       </c>
-    </row>
-    <row r="43" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E43" t="s">
+      <c r="F66" t="s">
+        <v>15</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E67" s="6">
         <v>59</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E44" t="s">
+      <c r="F67" t="s">
+        <v>78</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E68" s="6">
         <v>60</v>
       </c>
-    </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E45" t="s">
+      <c r="F68" t="s">
+        <v>13</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E69" s="6">
         <v>61</v>
       </c>
-    </row>
-    <row r="46" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E46" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E47" t="s">
+      <c r="F69" t="s">
+        <v>79</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="71" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E71" s="4">
         <v>62</v>
       </c>
-    </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E49" t="s">
+      <c r="F71" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="72" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E72" s="4">
         <v>63</v>
       </c>
-    </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E50" t="s">
+      <c r="F72" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="73" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E73" s="4">
         <v>64</v>
       </c>
-    </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E51" t="s">
+      <c r="F73" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="74" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E74" s="4">
         <v>65</v>
       </c>
-    </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E52" t="s">
+      <c r="F74" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="75" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E75" s="4">
         <v>66</v>
       </c>
-    </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E53" t="s">
+      <c r="F75" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="76" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E76" s="4">
         <v>67</v>
       </c>
-    </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E54" t="s">
+      <c r="F76" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="78" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E78" s="4">
         <v>68</v>
       </c>
-    </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E55" t="s">
+      <c r="F78" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="79" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E79" s="4">
         <v>69</v>
       </c>
-    </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E56" t="s">
+      <c r="F79" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E80" s="4">
         <v>70</v>
       </c>
-    </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E57" t="s">
+      <c r="F80" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E81" s="4">
         <v>71</v>
       </c>
-    </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E58" t="s">
+      <c r="F81" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="82" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E82" s="4">
         <v>72</v>
       </c>
-    </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E59" t="s">
+      <c r="F82" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="83" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E83" s="4">
         <v>73</v>
       </c>
-    </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E60" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E61" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E62" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E64" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E65" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E66" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E67" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E68" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E69" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E71" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E72" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E73" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E74" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E75" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E76" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E78" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E79" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E80" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E81" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E82" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E83" t="s">
+      <c r="F83" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>